<commit_message>
Menghapus koma dari data harga XAUUSD
</commit_message>
<xml_diff>
--- a/Preprocess Logam dan Minyak/XAG_USD.xlsx
+++ b/Preprocess Logam dan Minyak/XAG_USD.xlsx
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1303" workbookViewId="0">
+      <selection activeCell="D1324" sqref="D1324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
git push dan remote vscode error, tidak support
Membuat branch dan deploy program secara manual melalui github
</commit_message>
<xml_diff>
--- a/Preprocess Logam dan Minyak/XAG_USD.xlsx
+++ b/Preprocess Logam dan Minyak/XAG_USD.xlsx
@@ -2409,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A1303" workbookViewId="0">
+      <selection activeCell="D1324" sqref="D1324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>